<commit_message>
add doc for my experiment improvement
</commit_message>
<xml_diff>
--- a/report/Results summary.xlsx
+++ b/report/Results summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\__uni\Autoformer\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC11E5B-9DC9-402A-A2BC-E5A07DB229AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8659EEF-19DE-40CE-B954-20D6EDBE4C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0D0B57C7-4B5F-40EF-ADC9-7A98D33306A9}"/>
   </bookViews>
@@ -321,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -728,6 +734,8 @@
     <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1085,9 +1093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC49915-A8E7-4BB1-8812-E70BD6BDF81F}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,64 +1313,64 @@
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="17">
         <v>3</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="G8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="17">
         <v>9.9699999999999997E-2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="18">
         <v>0.2487</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="D9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="17">
         <v>9.2399999999999996E-2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="18">
         <v>0.22450000000000001</v>
       </c>
     </row>

</xml_diff>